<commit_message>
refactor: :recycle: update global.xlsx
</commit_message>
<xml_diff>
--- a/global.xlsx
+++ b/global.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="profile" sheetId="1" state="visible" r:id="rId2"/>
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2368" uniqueCount="1155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2384" uniqueCount="1159">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -5153,13 +5153,16 @@
     <t xml:space="preserve">On examination, the child has been found to have a skin, mouth or eye problem not reported by the caregiver, or not already assessed.</t>
   </si>
   <si>
+    <t xml:space="preserve">"Danger Signs" != true </t>
+  </si>
+  <si>
     <t xml:space="preserve">EmCare.B14S2.DE44</t>
   </si>
   <si>
     <t xml:space="preserve">The child has a skin problem</t>
   </si>
   <si>
-    <t xml:space="preserve">"Skin problem" != true and "Pain" != "Skin problem"</t>
+    <t xml:space="preserve">"Skin problem" != true and "Pain" != true</t>
   </si>
   <si>
     <t xml:space="preserve">EmCare.B14S2.DE45</t>
@@ -5281,7 +5284,7 @@
     <t xml:space="preserve">force-collection</t>
   </si>
   <si>
-    <t xml:space="preserve">Respiratory Rate Second Count Profile</t>
+    <t xml:space="preserve">Respiratory Rate (Second Count) (breaths per minute)</t>
   </si>
   <si>
     <t xml:space="preserve">o"Respiratory Rate (Second Count) (breaths per minute)"</t>
@@ -5291,6 +5294,18 @@
   </si>
   <si>
     <t xml:space="preserve">o"Fast Breathing"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Respiratory Rate (Second Count) (breaths per minute)".empty()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">o”AgeInMonths”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Respiratory Rate (Second Count) Not Possible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">o”Respiratory Rate (Second Count) Not Possible”</t>
   </si>
   <si>
     <t xml:space="preserve">EmCare.B24.G.DE01</t>
@@ -5480,7 +5495,7 @@
     <t xml:space="preserve">second</t>
   </si>
   <si>
-    <t xml:space="preserve">"AgeInMonths" &lt; 2 and ("Respiratory Rate profile" &gt;= 60 '{Breaths}/min' or "Respiratory Rate (breaths per minute)" &gt;= 60 '{Breaths}/min') and   "Respiratory Rate Second Count Profile".empty()</t>
+    <t xml:space="preserve">"AgeInMonths" &lt; 2 and ("Respiratory Rate profile" &gt;= 60 '{Breaths}/min' or "Respiratory Rate (breaths per minute)" &gt;= 60 '{Breaths}/min') and "Respiratory Rate (Second Count) (breaths per minute)".empty()</t>
   </si>
   <si>
     <t xml:space="preserve">EmCare.B24.G.DE03</t>
@@ -5601,9 +5616,6 @@
     <t xml:space="preserve">The child's second respiratory rate is not possible to measure</t>
   </si>
   <si>
-    <t xml:space="preserve"> "Respiratory Rate (Second Count) (breaths per minute)".empty()</t>
-  </si>
-  <si>
     <t xml:space="preserve">EmCare.B24.G.DE05</t>
   </si>
   <si>
@@ -5626,7 +5638,7 @@
     <t xml:space="preserve">fastbreathing-True</t>
   </si>
   <si>
-    <t xml:space="preserve">Fast Breathing </t>
+    <t xml:space="preserve">Fast Breathing True</t>
   </si>
   <si>
     <t xml:space="preserve">Fast breathing is auto-calculated based on the respiratory rate and the child's age: 
@@ -5664,14 +5676,14 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">"=true</t>
+      <t xml:space="preserve">" = true</t>
     </r>
   </si>
   <si>
     <t xml:space="preserve">fastbreathing-False</t>
   </si>
   <si>
-    <t xml:space="preserve">No Fast Breathing</t>
+    <t xml:space="preserve">Fast Breathing False</t>
   </si>
   <si>
     <r>
@@ -5702,7 +5714,7 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">"=false</t>
+      <t xml:space="preserve">" = false</t>
     </r>
   </si>
   <si>
@@ -7278,19 +7290,19 @@
   </sheetPr>
   <dimension ref="A1:AMJ97"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="I49" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="E29" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="I1" activeCellId="0" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="A49" activeCellId="0" sqref="A49"/>
-      <selection pane="bottomRight" activeCell="I52" activeCellId="0" sqref="I52"/>
+      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A29" activeCellId="0" sqref="A29"/>
+      <selection pane="bottomRight" activeCell="A30" activeCellId="0" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.45"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="11.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="45.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="34.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="50.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="36.36"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="11.54"/>
@@ -7612,6 +7624,9 @@
       <c r="H15" s="29" t="s">
         <v>876</v>
       </c>
+      <c r="L15" s="12" t="s">
+        <v>524</v>
+      </c>
       <c r="P15" s="71"/>
     </row>
     <row r="16" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7645,6 +7660,9 @@
       <c r="H17" s="29" t="s">
         <v>880</v>
       </c>
+      <c r="L17" s="12" t="s">
+        <v>524</v>
+      </c>
       <c r="P17" s="71"/>
     </row>
     <row r="18" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7660,6 +7678,9 @@
       <c r="H18" s="29" t="s">
         <v>882</v>
       </c>
+      <c r="L18" s="12" t="s">
+        <v>524</v>
+      </c>
       <c r="P18" s="71"/>
     </row>
     <row r="19" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7675,6 +7696,9 @@
       <c r="H19" s="29" t="s">
         <v>884</v>
       </c>
+      <c r="L19" s="12" t="s">
+        <v>524</v>
+      </c>
       <c r="P19" s="71"/>
     </row>
     <row r="20" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7690,6 +7714,9 @@
       <c r="H20" s="29" t="s">
         <v>886</v>
       </c>
+      <c r="L20" s="12" t="s">
+        <v>524</v>
+      </c>
       <c r="P20" s="71"/>
     </row>
     <row r="21" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7705,6 +7732,9 @@
       <c r="H21" s="29" t="s">
         <v>888</v>
       </c>
+      <c r="L21" s="12" t="s">
+        <v>524</v>
+      </c>
       <c r="P21" s="71"/>
     </row>
     <row r="22" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7719,6 +7749,9 @@
       <c r="F22" s="72"/>
       <c r="H22" s="29" t="s">
         <v>890</v>
+      </c>
+      <c r="L22" s="12" t="s">
+        <v>524</v>
       </c>
       <c r="P22" s="71"/>
     </row>
@@ -11185,10 +11218,10 @@
         <v>1077</v>
       </c>
       <c r="I73" s="29" t="s">
-        <v>1053</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1078</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="22.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
         <v>412</v>
       </c>
@@ -11196,16 +11229,16 @@
         <v>1075</v>
       </c>
       <c r="C74" s="47" t="s">
-        <v>1078</v>
+        <v>1079</v>
       </c>
       <c r="D74" s="123" t="s">
         <v>855</v>
       </c>
       <c r="E74" s="35" t="s">
-        <v>1079</v>
+        <v>1080</v>
       </c>
       <c r="I74" s="47" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="P74" s="124" t="s">
         <v>712</v>
@@ -11225,16 +11258,16 @@
         <v>1075</v>
       </c>
       <c r="C75" s="47" t="s">
-        <v>1081</v>
+        <v>1082</v>
       </c>
       <c r="D75" s="123" t="s">
-        <v>1082</v>
+        <v>1083</v>
       </c>
       <c r="E75" s="35" t="s">
-        <v>1082</v>
+        <v>1083</v>
       </c>
       <c r="I75" s="41" t="s">
-        <v>1083</v>
+        <v>1084</v>
       </c>
       <c r="P75" s="124" t="s">
         <v>712</v>
@@ -11254,16 +11287,16 @@
         <v>1075</v>
       </c>
       <c r="C76" s="47" t="s">
-        <v>1084</v>
+        <v>1085</v>
       </c>
       <c r="D76" s="123" t="s">
         <v>852</v>
       </c>
       <c r="E76" s="35" t="s">
-        <v>1085</v>
+        <v>1086</v>
       </c>
       <c r="I76" s="41" t="s">
-        <v>1086</v>
+        <v>1087</v>
       </c>
       <c r="P76" s="124" t="s">
         <v>712</v>
@@ -11277,20 +11310,20 @@
     </row>
     <row r="77" customFormat="false" ht="195" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
-        <v>1087</v>
+        <v>1088</v>
       </c>
       <c r="B77" s="29"/>
       <c r="C77" s="47" t="s">
-        <v>1088</v>
+        <v>1089</v>
       </c>
       <c r="D77" s="37" t="s">
         <v>301</v>
       </c>
       <c r="E77" s="47" t="s">
-        <v>1089</v>
+        <v>1090</v>
       </c>
       <c r="I77" s="47" t="s">
-        <v>1090</v>
+        <v>1091</v>
       </c>
       <c r="P77" s="115" t="s">
         <v>979</v>
@@ -11304,16 +11337,16 @@
     </row>
     <row r="78" customFormat="false" ht="103.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
-        <v>1091</v>
+        <v>1092</v>
       </c>
       <c r="C78" s="125" t="s">
-        <v>1092</v>
+        <v>1093</v>
       </c>
       <c r="D78" s="47" t="s">
         <v>315</v>
       </c>
       <c r="E78" s="105" t="s">
-        <v>1093</v>
+        <v>1094</v>
       </c>
       <c r="P78" s="115" t="s">
         <v>645</v>
@@ -11331,7 +11364,7 @@
       </c>
       <c r="B79" s="29"/>
       <c r="C79" s="47" t="s">
-        <v>1094</v>
+        <v>1095</v>
       </c>
       <c r="D79" s="31" t="s">
         <v>250</v>
@@ -11429,17 +11462,26 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AG15"/>
+  <dimension ref="A1:AG17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="1" style="1" width="11.54"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="11.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="21.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="31.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="41.27"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="6" style="1" width="11.54"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="11.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="30.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="48.13"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="13" min="10" style="1" width="11.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="60.78"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="15" style="1" width="11.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11525,7 +11567,7 @@
       <c r="D2" s="1"/>
       <c r="E2" s="72"/>
       <c r="F2" s="72" t="s">
-        <v>1095</v>
+        <v>1096</v>
       </c>
       <c r="P2" s="71"/>
     </row>
@@ -11535,21 +11577,21 @@
       </c>
       <c r="B3" s="78"/>
       <c r="C3" s="78" t="s">
-        <v>1096</v>
+        <v>1097</v>
       </c>
       <c r="D3" s="55"/>
       <c r="E3" s="55"/>
       <c r="F3" s="55"/>
       <c r="G3" s="71"/>
       <c r="H3" s="71" t="s">
-        <v>1097</v>
+        <v>1098</v>
       </c>
       <c r="I3" s="71"/>
       <c r="K3" s="71"/>
-      <c r="L3" s="71"/>
-      <c r="N3" s="71" t="s">
+      <c r="L3" s="71" t="s">
         <v>524</v>
       </c>
+      <c r="N3" s="0"/>
       <c r="O3" s="71"/>
       <c r="P3" s="71"/>
       <c r="Q3" s="71"/>
@@ -11563,40 +11605,41 @@
       <c r="Y3" s="71"/>
       <c r="Z3" s="71"/>
     </row>
-    <row r="4" s="12" customFormat="true" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="12" t="s">
         <v>30</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>1098</v>
+        <v>1099</v>
       </c>
       <c r="H4" s="126" t="s">
         <v>370</v>
       </c>
-      <c r="N4" s="12" t="s">
+      <c r="L4" s="12" t="s">
         <v>524</v>
       </c>
+      <c r="N4" s="0"/>
     </row>
     <row r="5" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="12" t="s">
         <v>470</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>1099</v>
+        <v>1100</v>
       </c>
       <c r="D5" s="55"/>
       <c r="E5" s="55"/>
       <c r="F5" s="55"/>
       <c r="G5" s="71"/>
       <c r="H5" s="12" t="s">
-        <v>1100</v>
+        <v>1101</v>
       </c>
       <c r="I5" s="71"/>
       <c r="K5" s="71"/>
-      <c r="L5" s="71"/>
-      <c r="N5" s="71" t="s">
+      <c r="L5" s="71" t="s">
         <v>524</v>
       </c>
+      <c r="N5" s="0"/>
       <c r="O5" s="71"/>
       <c r="P5" s="71"/>
       <c r="Q5" s="71"/>
@@ -11615,21 +11658,23 @@
         <v>30</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>1101</v>
+        <v>1102</v>
       </c>
       <c r="D6" s="55"/>
       <c r="E6" s="55"/>
       <c r="F6" s="55"/>
       <c r="G6" s="71"/>
       <c r="H6" s="12" t="s">
-        <v>1102</v>
-      </c>
-      <c r="I6" s="71"/>
+        <v>1103</v>
+      </c>
+      <c r="I6" s="71" t="s">
+        <v>1104</v>
+      </c>
       <c r="K6" s="71"/>
-      <c r="L6" s="71"/>
-      <c r="N6" s="71" t="s">
+      <c r="L6" s="71" t="s">
         <v>524</v>
       </c>
+      <c r="N6" s="0"/>
       <c r="O6" s="71"/>
       <c r="P6" s="71"/>
       <c r="Q6" s="71"/>
@@ -11644,106 +11689,127 @@
       <c r="Z6" s="71"/>
     </row>
     <row r="7" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="57"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="72"/>
-      <c r="F7" s="72"/>
+      <c r="A7" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="55" t="s">
+        <v>445</v>
+      </c>
+      <c r="D7" s="55"/>
+      <c r="E7" s="55"/>
+      <c r="F7" s="55"/>
+      <c r="G7" s="71"/>
+      <c r="H7" s="12" t="s">
+        <v>1105</v>
+      </c>
+      <c r="I7" s="71"/>
+      <c r="K7" s="71"/>
+      <c r="L7" s="71" t="s">
+        <v>524</v>
+      </c>
+      <c r="N7" s="0"/>
+      <c r="O7" s="71"/>
       <c r="P7" s="71"/>
-    </row>
-    <row r="8" s="12" customFormat="true" ht="312" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="57" t="s">
+      <c r="Q7" s="71"/>
+      <c r="R7" s="71"/>
+      <c r="S7" s="71"/>
+      <c r="T7" s="71"/>
+      <c r="U7" s="71"/>
+      <c r="V7" s="71"/>
+      <c r="W7" s="71"/>
+      <c r="X7" s="71"/>
+      <c r="Y7" s="71"/>
+      <c r="Z7" s="71"/>
+    </row>
+    <row r="8" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>1106</v>
+      </c>
+      <c r="D8" s="55"/>
+      <c r="E8" s="55"/>
+      <c r="F8" s="55"/>
+      <c r="G8" s="71"/>
+      <c r="H8" s="12" t="s">
+        <v>1107</v>
+      </c>
+      <c r="I8" s="71"/>
+      <c r="K8" s="71"/>
+      <c r="L8" s="71" t="s">
+        <v>524</v>
+      </c>
+      <c r="N8" s="0"/>
+      <c r="O8" s="71"/>
+      <c r="P8" s="71"/>
+      <c r="Q8" s="71"/>
+      <c r="R8" s="71"/>
+      <c r="S8" s="71"/>
+      <c r="T8" s="71"/>
+      <c r="U8" s="71"/>
+      <c r="V8" s="71"/>
+      <c r="W8" s="71"/>
+      <c r="X8" s="71"/>
+      <c r="Y8" s="71"/>
+      <c r="Z8" s="71"/>
+    </row>
+    <row r="9" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="57"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="72"/>
+      <c r="F9" s="72"/>
+      <c r="P9" s="71"/>
+    </row>
+    <row r="10" s="12" customFormat="true" ht="312" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="57" t="s">
         <v>470</v>
       </c>
-      <c r="C8" s="41" t="s">
-        <v>1103</v>
-      </c>
-      <c r="D8" s="66" t="s">
-        <v>1104</v>
-      </c>
-      <c r="E8" s="102" t="s">
-        <v>1105</v>
-      </c>
-      <c r="F8" s="72"/>
-      <c r="I8" s="12" t="s">
-        <v>1106</v>
-      </c>
-      <c r="L8" s="12" t="s">
-        <v>1107</v>
-      </c>
-      <c r="P8" s="34" t="s">
+      <c r="C10" s="41" t="s">
+        <v>1108</v>
+      </c>
+      <c r="D10" s="66" t="s">
+        <v>1109</v>
+      </c>
+      <c r="E10" s="102" t="s">
+        <v>1110</v>
+      </c>
+      <c r="F10" s="72"/>
+      <c r="I10" s="12" t="s">
+        <v>1111</v>
+      </c>
+      <c r="L10" s="12" t="s">
+        <v>1112</v>
+      </c>
+      <c r="P10" s="34" t="s">
         <v>707</v>
       </c>
-      <c r="Q8" s="1"/>
-      <c r="R8" s="34" t="s">
+      <c r="Q10" s="1"/>
+      <c r="R10" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="S8" s="34" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="12" t="s">
+      <c r="S10" s="34" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="12" t="s">
         <v>412</v>
       </c>
-      <c r="C9" s="41" t="s">
-        <v>1108</v>
-      </c>
-      <c r="D9" s="40" t="s">
-        <v>1109</v>
-      </c>
-      <c r="E9" s="127" t="s">
-        <v>1110</v>
-      </c>
-      <c r="I9" s="12" t="s">
-        <v>1111</v>
-      </c>
-      <c r="P9" s="34" t="s">
+      <c r="C11" s="41" t="s">
+        <v>1113</v>
+      </c>
+      <c r="D11" s="40" t="s">
+        <v>1114</v>
+      </c>
+      <c r="E11" s="127" t="s">
+        <v>1115</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>1116</v>
+      </c>
+      <c r="P11" s="34" t="s">
         <v>712</v>
-      </c>
-      <c r="R9" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="S9" s="34" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>548</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>1112</v>
-      </c>
-      <c r="D10" s="40"/>
-      <c r="E10" s="127"/>
-      <c r="I10" s="12" t="s">
-        <v>1113</v>
-      </c>
-      <c r="P10" s="34"/>
-      <c r="R10" s="34"/>
-      <c r="S10" s="34"/>
-    </row>
-    <row r="11" customFormat="false" ht="234" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="12" t="s">
-        <v>470</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>1112</v>
-      </c>
-      <c r="C11" s="41" t="s">
-        <v>1114</v>
-      </c>
-      <c r="D11" s="37" t="s">
-        <v>1115</v>
-      </c>
-      <c r="E11" s="38" t="s">
-        <v>1116</v>
-      </c>
-      <c r="I11" s="12" t="s">
-        <v>1117</v>
-      </c>
-      <c r="P11" s="34" t="s">
-        <v>707</v>
       </c>
       <c r="R11" s="34" t="s">
         <v>16</v>
@@ -11753,55 +11819,42 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="12" t="s">
-        <v>412</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>1112</v>
-      </c>
-      <c r="C12" s="41" t="s">
+      <c r="A12" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>1117</v>
+      </c>
+      <c r="D12" s="40"/>
+      <c r="E12" s="127"/>
+      <c r="I12" s="12" t="s">
         <v>1118</v>
       </c>
-      <c r="D12" s="40" t="s">
+      <c r="P12" s="34"/>
+      <c r="R12" s="34"/>
+      <c r="S12" s="34"/>
+    </row>
+    <row r="13" customFormat="false" ht="234" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="12" t="s">
+        <v>470</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>1117</v>
+      </c>
+      <c r="C13" s="41" t="s">
         <v>1119</v>
       </c>
-      <c r="E12" s="128" t="s">
+      <c r="D13" s="37" t="s">
         <v>1120</v>
       </c>
-      <c r="I12" s="12" t="s">
+      <c r="E13" s="38" t="s">
         <v>1121</v>
       </c>
-      <c r="P12" s="34" t="s">
-        <v>712</v>
-      </c>
-      <c r="R12" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="S12" s="34" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="142.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="41" t="s">
+      <c r="I13" s="12" t="s">
         <v>1122</v>
       </c>
-      <c r="D13" s="99" t="s">
-        <v>1123</v>
-      </c>
-      <c r="E13" s="88" t="s">
-        <v>1124</v>
-      </c>
-      <c r="G13" s="29" t="s">
-        <v>1125</v>
-      </c>
-      <c r="I13" s="12" t="s">
-        <v>1126</v>
-      </c>
       <c r="P13" s="34" t="s">
-        <v>607</v>
+        <v>707</v>
       </c>
       <c r="R13" s="34" t="s">
         <v>16</v>
@@ -11810,44 +11863,102 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="168.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="12" t="s">
+        <v>412</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>1117</v>
+      </c>
+      <c r="C14" s="41" t="s">
+        <v>1123</v>
+      </c>
+      <c r="D14" s="40" t="s">
+        <v>1124</v>
+      </c>
+      <c r="E14" s="128" t="s">
+        <v>1125</v>
+      </c>
+      <c r="I14" s="12" t="s">
+        <v>1104</v>
+      </c>
+      <c r="P14" s="34" t="s">
+        <v>712</v>
+      </c>
+      <c r="R14" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="S14" s="34" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="142.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="41" t="s">
+        <v>1126</v>
+      </c>
+      <c r="D15" s="99" t="s">
+        <v>1127</v>
+      </c>
+      <c r="E15" s="88" t="s">
+        <v>1128</v>
+      </c>
+      <c r="G15" s="29" t="s">
+        <v>1129</v>
+      </c>
+      <c r="I15" s="12" t="s">
+        <v>1130</v>
+      </c>
+      <c r="P15" s="34" t="s">
+        <v>607</v>
+      </c>
+      <c r="R15" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="S15" s="34" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="137.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12" t="s">
-        <v>1127</v>
-      </c>
-      <c r="D14" s="12" t="s">
-        <v>1128</v>
-      </c>
-      <c r="E14" s="88" t="s">
-        <v>1129</v>
-      </c>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12" t="s">
-        <v>1130</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="168.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="93" t="s">
+      <c r="B16" s="12"/>
+      <c r="C16" s="12" t="s">
+        <v>1131</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>1132</v>
+      </c>
+      <c r="E16" s="88" t="s">
+        <v>1133</v>
+      </c>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12" t="s">
+        <v>1134</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="137.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="93" t="s">
         <v>62</v>
       </c>
-      <c r="B15" s="93"/>
-      <c r="C15" s="12" t="s">
-        <v>1131</v>
-      </c>
-      <c r="D15" s="93" t="s">
-        <v>1132</v>
-      </c>
-      <c r="E15" s="88" t="s">
-        <v>1129</v>
-      </c>
-      <c r="G15" s="93"/>
-      <c r="H15" s="93"/>
-      <c r="I15" s="12" t="s">
+      <c r="B17" s="93"/>
+      <c r="C17" s="12" t="s">
+        <v>1135</v>
+      </c>
+      <c r="D17" s="93" t="s">
+        <v>1136</v>
+      </c>
+      <c r="E17" s="88" t="s">
         <v>1133</v>
+      </c>
+      <c r="G17" s="93"/>
+      <c r="H17" s="93"/>
+      <c r="I17" s="12" t="s">
+        <v>1137</v>
       </c>
     </row>
   </sheetData>
@@ -11869,7 +11980,7 @@
   <dimension ref="A1:AG9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11959,7 +12070,7 @@
       </c>
       <c r="E2" s="85"/>
       <c r="F2" s="72" t="s">
-        <v>1134</v>
+        <v>1138</v>
       </c>
       <c r="P2" s="71"/>
     </row>
@@ -12008,19 +12119,19 @@
         <v>470</v>
       </c>
       <c r="C4" s="47" t="s">
-        <v>1135</v>
+        <v>1139</v>
       </c>
       <c r="D4" s="35" t="s">
-        <v>1136</v>
+        <v>1140</v>
       </c>
       <c r="E4" s="96" t="s">
-        <v>1137</v>
+        <v>1141</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>1138</v>
+        <v>1142</v>
       </c>
       <c r="I4" s="29" t="s">
-        <v>1139</v>
+        <v>1143</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>704</v>
@@ -12046,16 +12157,16 @@
         <v>412</v>
       </c>
       <c r="C5" s="47" t="s">
-        <v>1140</v>
+        <v>1144</v>
       </c>
       <c r="D5" s="35" t="s">
-        <v>1141</v>
+        <v>1145</v>
       </c>
       <c r="E5" s="45" t="s">
         <v>710</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>1142</v>
+        <v>1146</v>
       </c>
       <c r="P5" s="71" t="s">
         <v>712</v>
@@ -12073,16 +12184,16 @@
         <v>470</v>
       </c>
       <c r="C6" s="47" t="s">
-        <v>1143</v>
+        <v>1147</v>
       </c>
       <c r="D6" s="31" t="s">
-        <v>1144</v>
+        <v>1148</v>
       </c>
       <c r="E6" s="96" t="s">
-        <v>1145</v>
+        <v>1149</v>
       </c>
       <c r="I6" s="29" t="s">
-        <v>1146</v>
+        <v>1150</v>
       </c>
       <c r="L6" s="1" t="s">
         <v>704</v>
@@ -12105,17 +12216,17 @@
         <v>406</v>
       </c>
       <c r="C7" s="47" t="s">
-        <v>1147</v>
+        <v>1151</v>
       </c>
       <c r="D7" s="36" t="s">
-        <v>1148</v>
+        <v>1152</v>
       </c>
       <c r="E7" s="35" t="s">
-        <v>1149</v>
+        <v>1153</v>
       </c>
       <c r="F7" s="34"/>
       <c r="G7" s="97" t="s">
-        <v>1150</v>
+        <v>1154</v>
       </c>
       <c r="L7" s="1" t="s">
         <v>524</v>
@@ -12135,17 +12246,17 @@
         <v>412</v>
       </c>
       <c r="C8" s="47" t="s">
-        <v>1151</v>
+        <v>1155</v>
       </c>
       <c r="D8" s="31" t="s">
-        <v>1152</v>
+        <v>1156</v>
       </c>
       <c r="E8" s="35" t="s">
-        <v>1153</v>
+        <v>1157</v>
       </c>
       <c r="F8" s="34"/>
       <c r="I8" s="1" t="s">
-        <v>1154</v>
+        <v>1158</v>
       </c>
       <c r="P8" s="71" t="s">
         <v>712</v>
@@ -12183,8 +12294,8 @@
   </sheetPr>
   <dimension ref="A1:H101"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A71" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B74" activeCellId="0" sqref="B74"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.6328125" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13876,7 +13987,7 @@
   <dimension ref="A1:X25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
+      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14416,8 +14527,8 @@
   </sheetPr>
   <dimension ref="A1:BA65"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.36328125" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17404,8 +17515,8 @@
   </sheetPr>
   <dimension ref="A1:AF22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A14" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E26" activeCellId="0" sqref="E26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I8" activeCellId="0" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17979,7 +18090,7 @@
   </sheetPr>
   <dimension ref="A1:AF19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C4" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -18552,7 +18663,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F3" activeCellId="0" sqref="F3"/>
+      <selection pane="bottomRight" activeCell="H5" activeCellId="0" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -19288,8 +19399,8 @@
   </sheetPr>
   <dimension ref="A1:AG24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>